<commit_message>
1. Monster -> NPC로 변경. 2. NPC Manger 수정.
</commit_message>
<xml_diff>
--- a/DOC/MapleStory/ToDo.xlsx
+++ b/DOC/MapleStory/ToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\Git\Wany_Project\DOC\MapleStory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E78647-8BF0-42CD-910F-8E0E0483A551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9342CE68-E58F-45C6-B5F3-5985F062D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{A46BA287-FEA7-49A3-B502-4A81FCEBF1B2}"/>
+    <workbookView xWindow="-25620" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{A46BA287-FEA7-49A3-B502-4A81FCEBF1B2}"/>
   </bookViews>
   <sheets>
     <sheet name="2022-09-29" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>Update date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,6 +143,10 @@
   </si>
   <si>
     <t>단축키 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스프라이트로 들고 있는 경우와 텍스처로 들고 있는 경우 동시에 고려 해야함</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,7 +520,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -525,7 +529,7 @@
     <col min="2" max="2" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -541,7 +545,7 @@
       </c>
       <c r="E2" s="2">
         <f ca="1">TODAY()</f>
-        <v>44833</v>
+        <v>44834</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -574,6 +578,9 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
1. UI_btn 추가 중 멈춤.
</commit_message>
<xml_diff>
--- a/DOC/MapleStory/ToDo.xlsx
+++ b/DOC/MapleStory/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\Git\Wany_Project\DOC\MapleStory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F7750A-28BB-401C-8A7A-D1E92803E985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26617C19-B36D-4179-8B4D-68BCDD5A86F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Update date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,6 +191,22 @@
   <si>
     <t>더블 점프 이펙트만 추가 완료, 
 collision Update에 따라 피격 될 때가 있고 안될 때가 있음.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스킬 2개 추가. (즉발형)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사운드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>맵 사운드 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타격 사운드 출력</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I16"/>
+  <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -834,6 +850,18 @@
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="2">
+        <v>44838</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.76527777777777783</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
@@ -866,6 +894,25 @@
       </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Button 테스트 완료.
</commit_message>
<xml_diff>
--- a/DOC/MapleStory/ToDo.xlsx
+++ b/DOC/MapleStory/ToDo.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\Git\Wany_Project\DOC\MapleStory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Git\Wany_Project\DOC\MapleStory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26617C19-B36D-4179-8B4D-68BCDD5A86F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="2022-09-29" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -213,7 +212,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,11 +581,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -616,7 +615,7 @@
       </c>
       <c r="E2" s="2">
         <f ca="1">TODAY()</f>
-        <v>44838</v>
+        <v>44839</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
@@ -865,54 +864,81 @@
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>19</v>
+        <v>40</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44839</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H14" s="2">
+        <v>44839</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.56041666666666667</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+      <c r="F15" s="2">
+        <v>44839</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="H15" s="2">
+        <v>44839</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.56041666666666667</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>9</v>
+      </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>